<commit_message>
Missing rows logic and tests
</commit_message>
<xml_diff>
--- a/tests/data.xlsx
+++ b/tests/data.xlsx
@@ -4,18 +4,19 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Regular Data" sheetId="1" r:id="rId1"/>
+    <sheet name="Missing Cells" sheetId="2" r:id="rId2"/>
+    <sheet name="Missing Rows" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="9">
   <si>
     <t>A1</t>
   </si>
@@ -385,7 +386,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
@@ -457,4 +458,41 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>